<commit_message>
ajuste nos graficos do projeto 2
</commit_message>
<xml_diff>
--- a/base_Projeto_integrado.xlsx
+++ b/base_Projeto_integrado.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafael.lucena\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafael.lucena\Documents\GitHub\Machine-Learning-Group-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4FBB7D-ED0A-4EDB-BD0B-4907B17439E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1516EC6E-4BD7-4CAC-B03A-F8AEC8A18148}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1869,9 +1869,7 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -1890,7 +1888,51 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1901,6 +1943,22 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{35B53701-19EF-4301-AF8B-3CA5DEAF9728}" name="Tabela1" displayName="Tabela1" ref="A1:G1048576" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+  <autoFilter ref="A1:G1048576" xr:uid="{7E71A07E-4328-4ABC-AF1D-018A6AA1504D}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{E56146E4-B102-4D11-8A10-FC1E11652A6E}" name="title"/>
+    <tableColumn id="2" xr3:uid="{0AFB3CBE-4600-4363-AFE9-29ED8744B7F1}" name="price"/>
+    <tableColumn id="3" xr3:uid="{1CB2F15C-28BA-4D78-B107-E6D9A2D713EC}" name="combustivel"/>
+    <tableColumn id="4" xr3:uid="{AC4E3DEB-1504-4517-8CAE-EA69168461A4}" name="cambio"/>
+    <tableColumn id="5" xr3:uid="{DD2B0AC3-305F-46CC-8481-D3F752012FBD}" name="km"/>
+    <tableColumn id="6" xr3:uid="{7E465C0A-1F07-45DE-9BD8-D6BAB606EE15}" name="modelo_base"/>
+    <tableColumn id="7" xr3:uid="{9EB060B5-AF69-42C7-AFC4-40992CB7AB30}" name="descricao_modelo"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2227,17 +2285,17 @@
   <dimension ref="A1:G324"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="50.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.90625" customWidth="1"/>
+    <col min="3" max="3" width="12.90625" customWidth="1"/>
     <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.08984375" customWidth="1"/>
     <col min="7" max="7" width="41.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9695,5 +9753,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>